<commit_message>
attack mitigation code added
</commit_message>
<xml_diff>
--- a/Matlab code/dataset_angle.xlsx
+++ b/Matlab code/dataset_angle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\NDSS_2023\Event triggered intersection\Event-triggered Intersection - Carla\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabbir92\Documents\GitHub\Trust_based_CBF\Matlab code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A509F72D-5A0A-4473-8455-0AF4CE10C1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8060F96-1897-464E-ADEF-1E9528D719A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{3E44235E-05CD-4E29-AF25-95F45ED84EE5}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="8170" xr2:uid="{3E44235E-05CD-4E29-AF25-95F45ED84EE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -388,9 +388,9 @@
       <selection sqref="A1:AGL25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>355.79705606696626</v>
       </c>
       <c r="BS3">
-        <v>351.96983172236401</v>
+        <v>351.96983172236384</v>
       </c>
       <c r="BT3">
         <v>351.53330013930207</v>
@@ -5844,10 +5844,10 @@
         <v>329.07242953994489</v>
       </c>
       <c r="BY3">
-        <v>328.91884871896616</v>
+        <v>328.9188487189669</v>
       </c>
       <c r="BZ3">
-        <v>328.881210721103</v>
+        <v>328.88121072110226</v>
       </c>
       <c r="CA3">
         <v>314.4711345608834</v>
@@ -8226,7 +8226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
@@ -8360,58 +8360,58 @@
         <v>89.861722174720626</v>
       </c>
       <c r="AS4">
-        <v>89.864210230667993</v>
+        <v>89.86421023066606</v>
       </c>
       <c r="AT4">
-        <v>89.864282289414177</v>
+        <v>89.86428228941611</v>
       </c>
       <c r="AU4">
         <v>89.864320774465455</v>
       </c>
       <c r="AV4">
-        <v>89.864339733124041</v>
+        <v>89.864339733122165</v>
       </c>
       <c r="AW4">
-        <v>89.864347584513212</v>
+        <v>89.864347584515087</v>
       </c>
       <c r="AX4">
-        <v>89.864351614474401</v>
+        <v>89.864351614474344</v>
       </c>
       <c r="AY4">
         <v>89.864351878911634</v>
       </c>
       <c r="AZ4">
-        <v>89.864351893062576</v>
+        <v>89.864351893064338</v>
       </c>
       <c r="BA4">
-        <v>89.864351895243999</v>
+        <v>89.864351895242237</v>
       </c>
       <c r="BB4">
         <v>89.864351895426694</v>
       </c>
       <c r="BC4">
-        <v>89.864351895454831</v>
+        <v>89.864351895456593</v>
       </c>
       <c r="BD4">
-        <v>89.864351895460516</v>
+        <v>89.864351895457162</v>
       </c>
       <c r="BE4">
-        <v>89.864351895459947</v>
+        <v>89.864351895461596</v>
       </c>
       <c r="BF4">
-        <v>89.864351895458128</v>
+        <v>89.864351895458185</v>
       </c>
       <c r="BG4">
         <v>89.864351895459833</v>
       </c>
       <c r="BH4">
-        <v>89.864351895461198</v>
+        <v>89.864351895459549</v>
       </c>
       <c r="BI4">
         <v>89.864351895460914</v>
       </c>
       <c r="BJ4">
-        <v>89.864351895459549</v>
+        <v>89.864351895461141</v>
       </c>
       <c r="BK4">
         <v>89.864351895459549</v>
@@ -8426,10 +8426,10 @@
         <v>89.864351895460118</v>
       </c>
       <c r="BO4">
-        <v>89.86435189545972</v>
+        <v>89.864351895461255</v>
       </c>
       <c r="BP4">
-        <v>89.864351895461198</v>
+        <v>89.864351895459663</v>
       </c>
       <c r="BQ4">
         <v>89.864351895458299</v>
@@ -8447,10 +8447,10 @@
         <v>89.864351895459436</v>
       </c>
       <c r="BV4">
-        <v>89.864351895459663</v>
+        <v>89.864351895461141</v>
       </c>
       <c r="BW4">
-        <v>89.864351895460288</v>
+        <v>89.86435189545881</v>
       </c>
       <c r="BX4">
         <v>89.864351895459492</v>
@@ -8498,10 +8498,10 @@
         <v>89.864351895459492</v>
       </c>
       <c r="CM4">
-        <v>89.864351895459492</v>
+        <v>89.864351895461084</v>
       </c>
       <c r="CN4">
-        <v>89.864351895458867</v>
+        <v>89.864351895457276</v>
       </c>
       <c r="CO4">
         <v>89.864351895460743</v>
@@ -8531,25 +8531,25 @@
         <v>113.31867992155196</v>
       </c>
       <c r="CX4">
-        <v>120.3804142788357</v>
+        <v>120.38041427883428</v>
       </c>
       <c r="CY4">
-        <v>132.60795266199324</v>
+        <v>132.60795266199443</v>
       </c>
       <c r="CZ4">
-        <v>146.15789899298102</v>
+        <v>146.15789899297749</v>
       </c>
       <c r="DA4">
-        <v>148.27133724235057</v>
+        <v>148.2713372423533</v>
       </c>
       <c r="DB4">
-        <v>169.15116970605607</v>
+        <v>169.15116970605288</v>
       </c>
       <c r="DC4">
-        <v>171.23317409850915</v>
+        <v>171.23317409851234</v>
       </c>
       <c r="DD4">
-        <v>171.47764002271333</v>
+        <v>171.47764002271356</v>
       </c>
       <c r="DE4">
         <v>179.01782957367345</v>
@@ -10838,7 +10838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -13450,7 +13450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -16062,7 +16062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0</v>
       </c>
@@ -16286,13 +16286,13 @@
         <v>181.52490319474262</v>
       </c>
       <c r="BW7">
-        <v>181.52490319474251</v>
+        <v>181.52490319473992</v>
       </c>
       <c r="BX7">
-        <v>181.52490319473904</v>
+        <v>181.52490319474157</v>
       </c>
       <c r="BY7">
-        <v>181.52490319474043</v>
+        <v>181.52490319474049</v>
       </c>
       <c r="BZ7">
         <v>181.52490319474069</v>
@@ -16304,19 +16304,19 @@
         <v>181.5249031947385</v>
       </c>
       <c r="CC7">
-        <v>181.52490319474057</v>
+        <v>181.52490319474313</v>
       </c>
       <c r="CD7">
-        <v>181.52490319474185</v>
+        <v>181.52490319473924</v>
       </c>
       <c r="CE7">
-        <v>181.52490319474168</v>
+        <v>181.52490319474163</v>
       </c>
       <c r="CF7">
-        <v>181.52490319474146</v>
+        <v>181.52490319474148</v>
       </c>
       <c r="CG7">
-        <v>181.524903194742</v>
+        <v>181.52490319474208</v>
       </c>
       <c r="CH7">
         <v>181.52490319474157</v>
@@ -16337,10 +16337,10 @@
         <v>181.63393551152097</v>
       </c>
       <c r="CN7">
-        <v>181.40347772639041</v>
+        <v>181.40347772638776</v>
       </c>
       <c r="CO7">
-        <v>181.50944596244756</v>
+        <v>181.50944596245014</v>
       </c>
       <c r="CP7">
         <v>181.41660353374479</v>
@@ -16352,7 +16352,7 @@
         <v>181.26013718927868</v>
       </c>
       <c r="CS7">
-        <v>181.13457727808543</v>
+        <v>181.1345772780854</v>
       </c>
       <c r="CT7">
         <v>180.80395017845339</v>
@@ -16361,7 +16361,7 @@
         <v>180.99271939674315</v>
       </c>
       <c r="CV7">
-        <v>180.61238834117799</v>
+        <v>180.61238834117802</v>
       </c>
       <c r="CW7">
         <v>180.57537747677506</v>
@@ -16370,10 +16370,10 @@
         <v>180.21202756075778</v>
       </c>
       <c r="CY7">
-        <v>179.7315420968938</v>
+        <v>179.73154209689631</v>
       </c>
       <c r="CZ7">
-        <v>179.62093225475178</v>
+        <v>179.62093225474928</v>
       </c>
       <c r="DA7">
         <v>179.60287570384025</v>
@@ -16382,10 +16382,10 @@
         <v>179.60037477945036</v>
       </c>
       <c r="DC7">
-        <v>179.6000640815306</v>
+        <v>179.60006408152788</v>
       </c>
       <c r="DD7">
-        <v>179.59996089583433</v>
+        <v>179.59996089583728</v>
       </c>
       <c r="DE7">
         <v>179.59995899637329</v>
@@ -16397,10 +16397,10 @@
         <v>179.59995840086276</v>
       </c>
       <c r="DH7">
-        <v>179.59995839047815</v>
+        <v>179.59995839047485</v>
       </c>
       <c r="DI7">
-        <v>179.59995838939767</v>
+        <v>179.59995838940108</v>
       </c>
       <c r="DJ7">
         <v>179.5999583892708</v>
@@ -18674,7 +18674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -21286,7 +21286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
@@ -21552,10 +21552,10 @@
         <v>2.4960041774022557E-2</v>
       </c>
       <c r="CK9">
-        <v>2.4960041775500486E-2</v>
+        <v>2.4960041772772001E-2</v>
       </c>
       <c r="CL9">
-        <v>2.4960041770327734E-2</v>
+        <v>2.4960041773113062E-2</v>
       </c>
       <c r="CM9">
         <v>2.4960041771123542E-2</v>
@@ -21570,25 +21570,25 @@
         <v>2.4960041774193087E-2</v>
       </c>
       <c r="CQ9">
-        <v>2.4960041771407759E-2</v>
+        <v>2.4960041774193087E-2</v>
       </c>
       <c r="CR9">
-        <v>2.4960041775329955E-2</v>
+        <v>2.4960041772544628E-2</v>
       </c>
       <c r="CS9">
-        <v>2.4960041768963492E-2</v>
+        <v>2.496004177174882E-2</v>
       </c>
       <c r="CT9">
-        <v>2.4960041775955233E-2</v>
+        <v>2.4960041773169905E-2</v>
       </c>
       <c r="CU9">
         <v>2.4960041770839325E-2</v>
       </c>
       <c r="CV9">
-        <v>2.4960041771691976E-2</v>
+        <v>2.4960041774534147E-2</v>
       </c>
       <c r="CW9">
-        <v>2.4960041772146724E-2</v>
+        <v>2.4960041769361396E-2</v>
       </c>
       <c r="CX9">
         <v>2.4960041773397279E-2</v>
@@ -21603,10 +21603,10 @@
         <v>1.8567702924087826E-2</v>
       </c>
       <c r="DB9">
-        <v>8.7765273258924026E-3</v>
+        <v>8.7765273287914169E-3</v>
       </c>
       <c r="DC9">
-        <v>1.5571580809137231E-4</v>
+        <v>1.5571580524920137E-4</v>
       </c>
       <c r="DD9">
         <v>9.8644205763775972E-6</v>
@@ -21630,10 +21630,10 @@
         <v>1.0788880899781361E-10</v>
       </c>
       <c r="DK9">
-        <v>8.7538865045644343E-12</v>
+        <v>5.8548721426632255E-12</v>
       </c>
       <c r="DL9">
-        <v>0</v>
+        <v>2.9558577807620168E-12</v>
       </c>
       <c r="DM9">
         <v>0</v>
@@ -21645,49 +21645,49 @@
         <v>359.65635416568557</v>
       </c>
       <c r="DP9">
-        <v>359.74594081598684</v>
+        <v>359.74594081598389</v>
       </c>
       <c r="DQ9">
-        <v>355.92453925139955</v>
+        <v>355.92453925140239</v>
       </c>
       <c r="DR9">
-        <v>352.85764041249206</v>
+        <v>352.85764041249814</v>
       </c>
       <c r="DS9">
-        <v>351.5872663475256</v>
+        <v>351.58726634752264</v>
       </c>
       <c r="DT9">
-        <v>351.50888401833072</v>
+        <v>351.50888401833095</v>
       </c>
       <c r="DU9">
-        <v>351.48442025570944</v>
+        <v>351.48442025571239</v>
       </c>
       <c r="DV9">
-        <v>351.48353210390422</v>
+        <v>351.48353210389854</v>
       </c>
       <c r="DW9">
-        <v>335.12000698000719</v>
+        <v>335.12000698002066</v>
       </c>
       <c r="DX9">
-        <v>328.89020726993289</v>
+        <v>328.89020726993368</v>
       </c>
       <c r="DY9">
-        <v>328.88237341133959</v>
+        <v>328.88237341134038</v>
       </c>
       <c r="DZ9">
-        <v>328.88006773115569</v>
+        <v>328.88006773115649</v>
       </c>
       <c r="EA9">
-        <v>323.29437742706421</v>
+        <v>323.29437742706608</v>
       </c>
       <c r="EB9">
-        <v>304.85593470221437</v>
+        <v>304.85593470222136</v>
       </c>
       <c r="EC9">
         <v>301.70230030025544</v>
       </c>
       <c r="ED9">
-        <v>301.16713716134768</v>
+        <v>301.16713716134734</v>
       </c>
       <c r="EE9">
         <v>301.06861731057791</v>
@@ -21696,31 +21696,31 @@
         <v>292.42000458623056</v>
       </c>
       <c r="EG9">
-        <v>281.51656535310383</v>
+        <v>281.51656535310701</v>
       </c>
       <c r="EH9">
-        <v>278.93193462791771</v>
+        <v>278.9319346279193</v>
       </c>
       <c r="EI9">
-        <v>278.27494799105767</v>
+        <v>278.27494799105818</v>
       </c>
       <c r="EJ9">
         <v>278.09125194617104</v>
       </c>
       <c r="EK9">
-        <v>278.04974141245987</v>
+        <v>278.04974141246191</v>
       </c>
       <c r="EL9">
-        <v>276.23928404832208</v>
+        <v>276.23928404832174</v>
       </c>
       <c r="EM9">
-        <v>270.30165179462779</v>
+        <v>270.30165179462938</v>
       </c>
       <c r="EN9">
-        <v>269.91477104717086</v>
+        <v>269.91477104717251</v>
       </c>
       <c r="EO9">
-        <v>269.87296667278758</v>
+        <v>269.87296667278599</v>
       </c>
       <c r="EP9">
         <v>269.86630721645975</v>
@@ -21753,7 +21753,7 @@
         <v>269.86435189550537</v>
       </c>
       <c r="EZ9">
-        <v>269.86435189547774</v>
+        <v>269.86435189547609</v>
       </c>
       <c r="FA9">
         <v>269.86435189545978</v>
@@ -21762,7 +21762,7 @@
         <v>269.86435189545978</v>
       </c>
       <c r="FC9">
-        <v>269.86435189545978</v>
+        <v>269.86435189546143</v>
       </c>
       <c r="FD9">
         <v>269.86435189545978</v>
@@ -21783,10 +21783,10 @@
         <v>269.86435189546143</v>
       </c>
       <c r="FJ9">
-        <v>269.86435189545978</v>
+        <v>269.86435189546143</v>
       </c>
       <c r="FK9">
-        <v>269.86435189545978</v>
+        <v>269.86435189545819</v>
       </c>
       <c r="FL9">
         <v>269.86435189545978</v>
@@ -21822,7 +21822,7 @@
         <v>269.86435189545819</v>
       </c>
       <c r="FW9">
-        <v>269.86435189545978</v>
+        <v>269.86435189546143</v>
       </c>
       <c r="FX9">
         <v>269.86435189546143</v>
@@ -21837,7 +21837,7 @@
         <v>269.86435189545978</v>
       </c>
       <c r="GB9">
-        <v>269.86435189546143</v>
+        <v>269.86435189545978</v>
       </c>
       <c r="GC9">
         <v>269.86435189545819</v>
@@ -21858,13 +21858,13 @@
         <v>269.86435189545978</v>
       </c>
       <c r="GI9">
-        <v>269.86435189545978</v>
+        <v>269.86435189545819</v>
       </c>
       <c r="GJ9">
         <v>269.86435189545978</v>
       </c>
       <c r="GK9">
-        <v>269.86435189545978</v>
+        <v>269.86435189546143</v>
       </c>
       <c r="GL9">
         <v>269.86435189545978</v>
@@ -21873,7 +21873,7 @@
         <v>269.86435189545978</v>
       </c>
       <c r="GN9">
-        <v>269.86435189545978</v>
+        <v>269.86435189546143</v>
       </c>
       <c r="GO9">
         <v>269.86433464783158</v>
@@ -21885,13 +21885,13 @@
         <v>269.86433464782993</v>
       </c>
       <c r="GR9">
-        <v>269.86433464783158</v>
+        <v>269.86433464782993</v>
       </c>
       <c r="GS9">
         <v>269.86433464783158</v>
       </c>
       <c r="GT9">
-        <v>269.86433464782993</v>
+        <v>269.86433464783158</v>
       </c>
       <c r="GU9">
         <v>269.86433464783158</v>
@@ -21909,7 +21909,7 @@
         <v>269.86433464782993</v>
       </c>
       <c r="GZ9">
-        <v>269.86433464783153</v>
+        <v>269.86433464783158</v>
       </c>
       <c r="HA9">
         <v>0</v>
@@ -23898,7 +23898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0</v>
       </c>
@@ -26510,7 +26510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -29122,7 +29122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -31734,7 +31734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0</v>
       </c>
@@ -34346,7 +34346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0</v>
       </c>
@@ -36958,7 +36958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0</v>
       </c>
@@ -39570,7 +39570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0</v>
       </c>
@@ -42182,7 +42182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0</v>
       </c>
@@ -44794,7 +44794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0</v>
       </c>
@@ -47406,7 +47406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0</v>
       </c>
@@ -50018,7 +50018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0</v>
       </c>
@@ -52630,7 +52630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0</v>
       </c>
@@ -55242,7 +55242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0</v>
       </c>
@@ -57854,7 +57854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0</v>
       </c>
@@ -60466,7 +60466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0</v>
       </c>
@@ -63078,7 +63078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:870" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:870" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0</v>
       </c>

</xml_diff>